<commit_message>
updated requirements and dockerfile
</commit_message>
<xml_diff>
--- a/Job_Hunt.xlsx
+++ b/Job_Hunt.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,12 +473,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://boards.greenhouse.io/foundation/jobs/4083425008?&amp;source=web3.career&amp;gh_src=web3.career</t>
+          <t>https://boards.greenhouse.io/lambda/jobs/6053055003</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>location matched</t>
+          <t>Remote but location not found</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -502,43 +502,6 @@
         </is>
       </c>
       <c r="G2" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://boards.greenhouse.io/singlestore/jobs/6125582</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>location matched</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
         <is>
           <t> </t>
         </is>

</xml_diff>

<commit_message>
default search sites added
</commit_message>
<xml_diff>
--- a/Job_Hunt.xlsx
+++ b/Job_Hunt.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,12 +473,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://boards.greenhouse.io/lambda/jobs/6053055003</t>
+          <t>https://jobs.lever.co/StubHub/098afbcb-6412-4646-903f-df11e51f7b33</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Remote but location not found</t>
+          <t>location matched</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -502,6 +502,191 @@
         </is>
       </c>
       <c r="G2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://jobs.boeing.com/category/engineering-software-jobs/185/2649/1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Posting Website</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://efds.fa.em5.oraclecloud.com/hcmUI/CandidateExperience/en/sites/CX_1/requisitions</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Posting Website</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://nvidia.wd5.myworkdayjobs.com/en-US/NVIDIAExternalCareerSite/job/US-CA-Santa-Clara/Senior-Software-Engineer---HPC_JR1983439?locationHierarchy1=2fcb99c455831013ea52fb338f2932d8</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>location matched</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>https://globalcareers-cotiviti.icims.com/jobs/12369/software-engineer/job?mobile=false&amp;width=1100&amp;height=500&amp;bga=true&amp;needsRedirect=false&amp;jan1offset=330&amp;jun1offset=330</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Posting Website</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>https://cooperative-sea-1e8.notion.site/d52db741a85748aead2235e7376f1974?v=902e7ec4bf28466f86dd89c8e9084427&amp;pvs=74</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Posting Website</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t> </t>
         </is>

</xml_diff>